<commit_message>
society import data feature improvement - area, subarea, city, state fixes
</commit_message>
<xml_diff>
--- a/coreapi/coreapi/v0/society_data.xlsx
+++ b/coreapi/coreapi/v0/society_data.xlsx
@@ -121,7 +121,7 @@
     <t xml:space="preserve">HR</t>
   </si>
   <si>
-    <t xml:space="preserve">KSH</t>
+    <t xml:space="preserve">ASD</t>
   </si>
   <si>
     <t xml:space="preserve">manager</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">Choco Pie</t>
   </si>
   <si>
-    <t xml:space="preserve">MIT</t>
+    <t xml:space="preserve">ZXC</t>
   </si>
 </sst>
 </file>
@@ -258,8 +258,8 @@
   </sheetPr>
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z1" activeCellId="0" sqref="Z1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,7 +445,7 @@
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="22.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
supplier_status and comments added to supplier society import functionality
</commit_message>
<xml_diff>
--- a/coreapi/coreapi/v0/society_data.xlsx
+++ b/coreapi/coreapi/v0/society_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t xml:space="preserve">Society Name</t>
   </si>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">HR</t>
   </si>
   <si>
-    <t xml:space="preserve">ASD</t>
+    <t xml:space="preserve">QWE</t>
   </si>
   <si>
     <t xml:space="preserve">manager</t>
@@ -148,10 +148,22 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
+    <t xml:space="preserve">Tapped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manager seems to be friendly</t>
+  </si>
+  <si>
     <t xml:space="preserve">Choco Pie</t>
   </si>
   <si>
     <t xml:space="preserve">ZXC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LetterGiven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manager is not friendly</t>
   </si>
 </sst>
 </file>
@@ -258,8 +270,8 @@
   </sheetPr>
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -268,7 +280,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.39"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="21" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="12.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="77.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,12 +457,16 @@
       <c r="AA2" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
+      <c r="AB2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
@@ -459,7 +478,7 @@
         <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>401105</v>
@@ -527,8 +546,12 @@
       <c r="AA3" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
+      <c r="AB3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
final changes for adding inventory summary in society import
</commit_message>
<xml_diff>
--- a/coreapi/coreapi/v0/society_data.xlsx
+++ b/coreapi/coreapi/v0/society_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t xml:space="preserve">Society Name</t>
   </si>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">Stall Allowed(Y/N)</t>
   </si>
   <si>
+    <t xml:space="preserve">Total Stall Count</t>
+  </si>
+  <si>
     <t xml:space="preserve">Poster Allowed NB</t>
   </si>
   <si>
@@ -91,7 +94,13 @@
     <t xml:space="preserve">Poster Allowed Lift</t>
   </si>
   <si>
-    <t xml:space="preserve">Door to Door Flier Allowed(Y/N)</t>
+    <t xml:space="preserve">Lift Per Tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flier Allowed(Y/N)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flier Frequency</t>
   </si>
   <si>
     <t xml:space="preserve">Stall Price(Small-1day)</t>
@@ -121,7 +130,7 @@
     <t xml:space="preserve">HR</t>
   </si>
   <si>
-    <t xml:space="preserve">QWE</t>
+    <t xml:space="preserve">ABC</t>
   </si>
   <si>
     <t xml:space="preserve">manager</t>
@@ -157,7 +166,7 @@
     <t xml:space="preserve">Choco Pie</t>
   </si>
   <si>
-    <t xml:space="preserve">ZXC</t>
+    <t xml:space="preserve">ADF</t>
   </si>
   <si>
     <t xml:space="preserve">LetterGiven</t>
@@ -268,25 +277,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="21" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="12.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="12.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="33" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="77.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="55.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -373,23 +383,32 @@
       </c>
       <c r="AC1" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>401105</v>
@@ -407,78 +426,87 @@
         <v>918</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="O2" s="1" t="n">
         <v>9090909090</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="S2" s="1" t="n">
         <v>2000302202</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V2" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="X2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y2" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="2" t="n">
         <v>3000</v>
       </c>
-      <c r="Z2" s="2" t="n">
+      <c r="AC2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="AA2" s="2" t="n">
+      <c r="AD2" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="AB2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>43</v>
+      <c r="AE2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>401105</v>
@@ -496,61 +524,70 @@
         <v>918</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="O3" s="1" t="n">
         <v>9090909090</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="S3" s="1" t="n">
         <v>2000302202</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V3" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="X3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y3" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="2" t="n">
         <v>3000</v>
       </c>
-      <c r="Z3" s="2" t="n">
+      <c r="AC3" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="AA3" s="2" t="n">
+      <c r="AD3" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="AB3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>47</v>
+      <c r="AE3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>